<commit_message>
Add sample collecting source
aware inconsistent name in traits #20
</commit_message>
<xml_diff>
--- a/metadata/Unit.xlsx
+++ b/metadata/Unit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marse\seadrive_root\Tien-Che\My Libraries\PhD_Tien\Project\Briwecs\BRIWECS_Data_Publication\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F52F15-7E27-46D9-BAB5-56602898F4B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823121D8-CC4D-4442-97CC-1DE69D27CA2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26865" windowHeight="8730" xr2:uid="{150D253A-C752-4639-9B69-1AA57574B26B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>Full name</t>
   </si>
@@ -282,6 +282,15 @@
   </si>
   <si>
     <t>% spike</t>
+  </si>
+  <si>
+    <t>sample source</t>
+  </si>
+  <si>
+    <t>biomass 50 cm cut</t>
+  </si>
+  <si>
+    <t>whole plot</t>
   </si>
 </sst>
 </file>
@@ -313,12 +322,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -353,10 +368,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F855A5-9A51-4B9F-9990-3A1DFD42927D}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +701,7 @@
     <col min="3" max="4" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,8 +711,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -705,8 +725,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -716,8 +739,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -727,8 +753,11 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -738,8 +767,11 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -749,8 +781,11 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -760,8 +795,11 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -771,8 +809,11 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -782,8 +823,11 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -793,8 +837,11 @@
       <c r="C10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -804,8 +851,11 @@
       <c r="C11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -815,8 +865,11 @@
       <c r="C12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -826,8 +879,11 @@
       <c r="C13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -837,8 +893,11 @@
       <c r="C14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -848,8 +907,11 @@
       <c r="C15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -859,8 +921,11 @@
       <c r="C16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -870,8 +935,11 @@
       <c r="C17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -881,8 +949,11 @@
       <c r="C18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -892,8 +963,11 @@
       <c r="C19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -903,8 +977,11 @@
       <c r="C20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -914,8 +991,11 @@
       <c r="C21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -925,16 +1005,22 @@
       <c r="C22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
       <c r="B23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -944,8 +1030,11 @@
       <c r="C24" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -955,8 +1044,11 @@
       <c r="C25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -965,6 +1057,9 @@
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update unit and abbreviaiton
</commit_message>
<xml_diff>
--- a/metadata/Unit.xlsx
+++ b/metadata/Unit.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marse\seadrive_root\Tien-Che\My Libraries\PhD_Tien\Project\Briwecs\BRIWECS_Data_Publication\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seafile\Tien-Che_1\My Libraries\PhD_Tien\Project\Briwecs\BRIWECS_Data_Publication\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FFFF13-09B8-466E-B8FC-39D7B25B5BF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26865" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26865" windowHeight="9675"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t>Full.name</t>
   </si>
@@ -112,15 +111,6 @@
     <t>Protein_yield</t>
   </si>
   <si>
-    <t xml:space="preserve">dt/ha </t>
-  </si>
-  <si>
-    <t>g/m2</t>
-  </si>
-  <si>
-    <t>#/m2</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -236,12 +226,45 @@
   </si>
   <si>
     <t>leaf rust caused by Puccinia triticina eriks.</t>
+  </si>
+  <si>
+    <t>abbrev</t>
+  </si>
+  <si>
+    <t>GY</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>GpS</t>
+  </si>
+  <si>
+    <t>GN</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>Shoot</t>
+  </si>
+  <si>
+    <t>dt/ha</t>
+  </si>
+  <si>
+    <t>g/m^2</t>
+  </si>
+  <si>
+    <t>#/m^2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -586,19 +609,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,367 +638,388 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -983,61 +1028,73 @@
         <v>#N/A</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
+      </c>
+      <c r="F26" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the important information that both seedyields are standardized to 100% dry matter. This is important, because in wheat often 86% is used.
</commit_message>
<xml_diff>
--- a/metadata/Unit.xlsx
+++ b/metadata/Unit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marse\seadrive_root\Tien-Che\My Libraries\PhD_Tien\Project\Briwecs\BRIWECS_Data_Publication\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillrose/Library/Mobile Documents/com~apple~CloudDocs/iCloud Daten/Arbeit/R-Projects/Git_Repositories/BRIWECS_Data_Publication/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDD7937-5A12-4DC0-B856-729D39DD5B23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4278468-DC32-E641-BA08-F39A39CD60B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26865" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30960" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
   <si>
     <t>Full.name</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t xml:space="preserve">thousand grain weight </t>
+  </si>
+  <si>
+    <t>dt/ha @100% dry mass</t>
+  </si>
+  <si>
+    <t>g/m^2 @100% dry mass</t>
   </si>
 </sst>
 </file>
@@ -318,9 +324,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,7 +364,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -464,7 +470,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -606,7 +612,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -617,17 +623,18 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.85546875" customWidth="1"/>
-    <col min="2" max="3" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="54.83203125" customWidth="1"/>
+    <col min="2" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +654,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -655,7 +662,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
         <v>36</v>
@@ -667,7 +674,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -675,7 +682,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
         <v>37</v>
@@ -684,7 +691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -704,7 +711,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -724,7 +731,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -744,7 +751,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -761,7 +768,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -781,7 +788,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -798,7 +805,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -815,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -832,7 +839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -849,7 +856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -866,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -883,7 +890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -900,7 +907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -917,7 +924,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -934,7 +941,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -951,7 +958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -968,7 +975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -985,7 +992,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1022,7 +1029,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1042,7 +1049,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1062,7 +1069,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1082,7 +1089,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>54</v>
       </c>

</xml_diff>